<commit_message>
Fixed GPT and adjustments
</commit_message>
<xml_diff>
--- a/Plans/Parts1.xlsx
+++ b/Plans/Parts1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grabinski.ma\Documents\GitHub\argon-dashboard-django\Plans\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikey\OneDrive\Documents\GitHub\MyResume\argon-dashboard-django\Plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043CE51E-2BAA-41B0-9697-A759E59E08FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A125DE34-7911-4D82-BCF9-4CDD49F686E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-6855" windowWidth="16440" windowHeight="28440" activeTab="1" xr2:uid="{AF8C979F-4DE1-4006-B607-399B4980CA4A}"/>
+    <workbookView xWindow="5295" yWindow="1155" windowWidth="13980" windowHeight="9750" activeTab="1" xr2:uid="{AF8C979F-4DE1-4006-B607-399B4980CA4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="202">
   <si>
     <t>Material</t>
   </si>
@@ -634,13 +634,16 @@
     <t>material cost incudle delivery and labour expect for trovel clean</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t xml:space="preserve">Excavation </t>
   </si>
   <si>
     <t>Excavator</t>
+  </si>
+  <si>
+    <t>Standard Truss - 4/12 (16' - 40')</t>
+  </si>
+  <si>
+    <t>250 each</t>
   </si>
 </sst>
 </file>
@@ -837,7 +840,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -856,7 +859,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -865,7 +867,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -884,9 +885,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -924,7 +925,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1030,7 +1031,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1172,7 +1173,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3007,15 +3008,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{668F61F5-DC84-4AC1-98B9-A5B51ED6513D}">
-  <dimension ref="A3:L40"/>
+  <dimension ref="A3:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" customWidth="1"/>
     <col min="5" max="5" width="63.42578125" customWidth="1"/>
     <col min="7" max="7" width="3.42578125" customWidth="1"/>
@@ -3045,24 +3046,24 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="22" t="s">
-        <v>199</v>
+      <c r="B8" s="21" t="s">
+        <v>198</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="12"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="19" t="s">
         <v>195</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="20" t="s">
         <v>196</v>
       </c>
       <c r="L9" t="s">
@@ -3071,47 +3072,40 @@
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14">
+        <v>199</v>
+      </c>
+      <c r="D10">
         <v>40</v>
       </c>
-      <c r="E10" s="15"/>
+      <c r="E10" s="14"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="13"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="15"/>
+      <c r="E11" s="14"/>
       <c r="L11" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="15"/>
+      <c r="E12" s="14"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="13"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="15"/>
+      <c r="E13" s="14"/>
     </row>
     <row r="14" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="16"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="18"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="17"/>
       <c r="L14" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="16" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="21" t="s">
         <v>184</v>
       </c>
       <c r="C17" s="11"/>
@@ -3122,16 +3116,16 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="19" t="s">
         <v>195</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="E18" s="20" t="s">
         <v>196</v>
       </c>
     </row>
@@ -3139,21 +3133,19 @@
       <c r="B19" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C19">
         <v>7000</v>
       </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="15"/>
+      <c r="E19" s="14"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B20" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C20">
         <v>3750</v>
       </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="14" t="s">
         <v>197</v>
       </c>
     </row>
@@ -3164,74 +3156,110 @@
       <c r="B21" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="15"/>
+      <c r="E21" s="14"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B22" s="13"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="15"/>
+      <c r="E22" s="14"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B23" s="13"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="15"/>
+      <c r="E23" s="14"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B24" s="13"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="15"/>
+      <c r="E24" s="14"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B25" s="13"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="15"/>
+      <c r="E25" s="14"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B26" s="13"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="15"/>
+      <c r="E26" s="14"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B27" s="13"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="15"/>
+      <c r="E27" s="14"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B28" s="13"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="15"/>
+      <c r="E28" s="14"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B29" s="13"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="15"/>
+      <c r="E29" s="14"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B30" s="13"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="15"/>
+      <c r="E30" s="14"/>
     </row>
     <row r="31" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="16"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="18"/>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" s="23" t="s">
-        <v>198</v>
-      </c>
+      <c r="B31" s="15"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="17"/>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="12"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="C37">
+        <v>9350</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="13"/>
+      <c r="E38" s="14"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>193</v>
+      </c>
+      <c r="B39" s="13"/>
+      <c r="E39" s="14"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="13"/>
+      <c r="E40" s="14"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="13"/>
+      <c r="E41" s="14"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="13"/>
+      <c r="E42" s="14"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="13"/>
+      <c r="E43" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed model choice and ggts lib
</commit_message>
<xml_diff>
--- a/Plans/Parts1.xlsx
+++ b/Plans/Parts1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikey\OneDrive\Documents\GitHub\MyResume\argon-dashboard-django\Plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A125DE34-7911-4D82-BCF9-4CDD49F686E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F89A41-2572-4E39-AC57-A93245166CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5295" yWindow="1155" windowWidth="13980" windowHeight="9750" activeTab="1" xr2:uid="{AF8C979F-4DE1-4006-B607-399B4980CA4A}"/>
+    <workbookView xWindow="1740" yWindow="990" windowWidth="13980" windowHeight="9750" activeTab="1" xr2:uid="{AF8C979F-4DE1-4006-B607-399B4980CA4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -643,7 +643,7 @@
     <t>Standard Truss - 4/12 (16' - 40')</t>
   </si>
   <si>
-    <t>250 each</t>
+    <t>145 each at mendards</t>
   </si>
 </sst>
 </file>
@@ -3010,8 +3010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{668F61F5-DC84-4AC1-98B9-A5B51ED6513D}">
   <dimension ref="A3:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3228,7 +3228,7 @@
         <v>200</v>
       </c>
       <c r="C37">
-        <v>9350</v>
+        <v>5500</v>
       </c>
       <c r="E37" s="14" t="s">
         <v>201</v>

</xml_diff>